<commit_message>
uploadの戻り値変更 Promise<any> -> Promise<any[]> Robot の  findByRobotName(name: string) の戻り値を変更 any -> Promise<any> Testケースのエラーログ出力を微調整
</commit_message>
<xml_diff>
--- a/src/services/templates/templateMachines.xlsx
+++ b/src/services/templates/templateMachines.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/masatomix/git/uipath-orchestrator-api-node/src/services/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467FC8CE-0630-AC4C-8453-1CFC461C1584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B947140-6064-7440-89AC-4D67AC08DECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33620" yWindow="6540" windowWidth="33600" windowHeight="9180" xr2:uid="{E608587B-B4D7-AC47-9EA0-EDA90FF582D2}"/>
+    <workbookView xWindow="-39100" yWindow="4280" windowWidth="33600" windowHeight="9180" xr2:uid="{E608587B-B4D7-AC47-9EA0-EDA90FF582D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -585,10 +585,10 @@
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -616,7 +616,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.140625" defaultRowHeight="20"/>
@@ -639,10 +639,10 @@
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">

</xml_diff>